<commit_message>
css override + typo
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petrkoci/code/nemocnice-personal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B6DB82-EDD8-F64A-A45C-F19E0A3341B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDF9B6E-49D6-F24B-8F80-ECEE146429F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="322">
   <si>
     <t>Thomayerova nemocnice</t>
   </si>
@@ -988,6 +988,9 @@
   </si>
   <si>
     <t>6 fyzio + 2 laboranti</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="M86" sqref="A1:M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1431,6 +1434,9 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="J3" t="s">
+        <v>321</v>
+      </c>
       <c r="K3" t="s">
         <v>128</v>
       </c>
@@ -1463,6 +1469,12 @@
       <c r="H4">
         <v>10</v>
       </c>
+      <c r="J4" t="s">
+        <v>321</v>
+      </c>
+      <c r="L4" t="s">
+        <v>321</v>
+      </c>
       <c r="M4" t="s">
         <v>12</v>
       </c>
@@ -1591,6 +1603,9 @@
       <c r="J8">
         <v>21</v>
       </c>
+      <c r="L8" t="s">
+        <v>321</v>
+      </c>
       <c r="M8" t="s">
         <v>14</v>
       </c>
@@ -1649,6 +1664,9 @@
       <c r="H10">
         <v>7</v>
       </c>
+      <c r="J10" t="s">
+        <v>321</v>
+      </c>
       <c r="L10">
         <v>12</v>
       </c>
@@ -1975,6 +1993,12 @@
       <c r="H20">
         <v>20</v>
       </c>
+      <c r="J20" t="s">
+        <v>321</v>
+      </c>
+      <c r="L20" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1998,6 +2022,12 @@
       <c r="H21">
         <v>7</v>
       </c>
+      <c r="J21" t="s">
+        <v>321</v>
+      </c>
+      <c r="L21" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -2021,6 +2051,12 @@
       <c r="H22">
         <v>8</v>
       </c>
+      <c r="J22" t="s">
+        <v>321</v>
+      </c>
+      <c r="L22" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -2044,6 +2080,12 @@
       <c r="H23">
         <v>5</v>
       </c>
+      <c r="J23" t="s">
+        <v>321</v>
+      </c>
+      <c r="L23" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2067,6 +2109,12 @@
       <c r="H24">
         <v>13</v>
       </c>
+      <c r="J24" t="s">
+        <v>321</v>
+      </c>
+      <c r="L24" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -2102,6 +2150,9 @@
       <c r="K25" t="s">
         <v>159</v>
       </c>
+      <c r="L25" t="s">
+        <v>321</v>
+      </c>
       <c r="M25" t="s">
         <v>23</v>
       </c>
@@ -2140,6 +2191,9 @@
       <c r="K26" t="s">
         <v>159</v>
       </c>
+      <c r="L26" t="s">
+        <v>321</v>
+      </c>
       <c r="M26" t="s">
         <v>23</v>
       </c>
@@ -2178,6 +2232,9 @@
       <c r="K27" t="s">
         <v>159</v>
       </c>
+      <c r="L27" t="s">
+        <v>321</v>
+      </c>
       <c r="M27" t="s">
         <v>23</v>
       </c>
@@ -2216,6 +2273,9 @@
       <c r="K28" t="s">
         <v>159</v>
       </c>
+      <c r="L28" t="s">
+        <v>321</v>
+      </c>
       <c r="M28" t="s">
         <v>23</v>
       </c>
@@ -2254,6 +2314,9 @@
       <c r="K29" t="s">
         <v>159</v>
       </c>
+      <c r="L29" t="s">
+        <v>321</v>
+      </c>
       <c r="M29" t="s">
         <v>23</v>
       </c>
@@ -2280,6 +2343,9 @@
       <c r="H30">
         <v>23</v>
       </c>
+      <c r="J30" t="s">
+        <v>321</v>
+      </c>
       <c r="L30">
         <v>31</v>
       </c>
@@ -2309,6 +2375,9 @@
       <c r="H31">
         <v>15</v>
       </c>
+      <c r="J31" t="s">
+        <v>321</v>
+      </c>
       <c r="L31">
         <v>21</v>
       </c>
@@ -2434,6 +2503,9 @@
       <c r="K35" t="s">
         <v>117</v>
       </c>
+      <c r="L35" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -2469,6 +2541,9 @@
       <c r="K36" t="s">
         <v>117</v>
       </c>
+      <c r="L36" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -2504,6 +2579,9 @@
       <c r="K37" t="s">
         <v>117</v>
       </c>
+      <c r="L37" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -2539,6 +2617,9 @@
       <c r="K38" t="s">
         <v>117</v>
       </c>
+      <c r="L38" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -2574,6 +2655,9 @@
       <c r="K39" t="s">
         <v>117</v>
       </c>
+      <c r="L39" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -2609,6 +2693,9 @@
       <c r="K40" t="s">
         <v>117</v>
       </c>
+      <c r="L40" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -2635,6 +2722,9 @@
       <c r="J41">
         <v>0</v>
       </c>
+      <c r="L41" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -2661,6 +2751,9 @@
       <c r="J42">
         <v>0</v>
       </c>
+      <c r="L42" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -2687,6 +2780,9 @@
       <c r="J43">
         <v>0</v>
       </c>
+      <c r="L43" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -2713,6 +2809,9 @@
       <c r="J44">
         <v>0</v>
       </c>
+      <c r="L44" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -2739,6 +2838,9 @@
       <c r="J45">
         <v>2</v>
       </c>
+      <c r="L45" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -2765,6 +2867,9 @@
       <c r="J46">
         <v>3</v>
       </c>
+      <c r="L46" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -2791,6 +2896,9 @@
       <c r="J47">
         <v>3</v>
       </c>
+      <c r="L47" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2817,6 +2925,9 @@
       <c r="J48">
         <v>0</v>
       </c>
+      <c r="L48" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -2843,6 +2954,9 @@
       <c r="J49">
         <v>4</v>
       </c>
+      <c r="L49" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -2866,6 +2980,12 @@
       <c r="H50">
         <v>9</v>
       </c>
+      <c r="J50" t="s">
+        <v>321</v>
+      </c>
+      <c r="L50" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -2976,8 +3096,17 @@
       <c r="E54" t="s">
         <v>237</v>
       </c>
+      <c r="F54" t="s">
+        <v>321</v>
+      </c>
       <c r="H54">
         <v>10</v>
+      </c>
+      <c r="J54" t="s">
+        <v>321</v>
+      </c>
+      <c r="L54" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -3034,6 +3163,9 @@
       <c r="J56">
         <v>8</v>
       </c>
+      <c r="L56" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -3092,6 +3224,9 @@
       <c r="J58">
         <v>11</v>
       </c>
+      <c r="L58" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -3118,6 +3253,9 @@
       <c r="J59">
         <v>3</v>
       </c>
+      <c r="L59" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
@@ -3144,6 +3282,9 @@
       <c r="J60">
         <v>6</v>
       </c>
+      <c r="L60" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -3161,14 +3302,26 @@
       <c r="E61" t="s">
         <v>256</v>
       </c>
+      <c r="F61" t="s">
+        <v>321</v>
+      </c>
       <c r="G61" t="s">
         <v>252</v>
       </c>
+      <c r="H61" t="s">
+        <v>321</v>
+      </c>
       <c r="I61" t="s">
         <v>252</v>
       </c>
+      <c r="J61" t="s">
+        <v>321</v>
+      </c>
       <c r="K61" t="s">
         <v>252</v>
+      </c>
+      <c r="L61" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -3187,11 +3340,20 @@
       <c r="E62" t="s">
         <v>259</v>
       </c>
+      <c r="F62" t="s">
+        <v>321</v>
+      </c>
       <c r="G62" t="s">
         <v>252</v>
       </c>
+      <c r="H62" t="s">
+        <v>321</v>
+      </c>
       <c r="I62" t="s">
         <v>252</v>
+      </c>
+      <c r="J62" t="s">
+        <v>321</v>
       </c>
       <c r="K62" t="s">
         <v>252</v>
@@ -3222,6 +3384,9 @@
       <c r="H63">
         <v>7</v>
       </c>
+      <c r="J63" t="s">
+        <v>321</v>
+      </c>
       <c r="L63">
         <v>14</v>
       </c>
@@ -3242,14 +3407,26 @@
       <c r="E64" t="s">
         <v>263</v>
       </c>
+      <c r="F64" t="s">
+        <v>321</v>
+      </c>
       <c r="G64" t="s">
         <v>252</v>
       </c>
+      <c r="H64" t="s">
+        <v>321</v>
+      </c>
       <c r="I64" t="s">
         <v>252</v>
       </c>
+      <c r="J64" t="s">
+        <v>321</v>
+      </c>
       <c r="K64" t="s">
         <v>252</v>
+      </c>
+      <c r="L64" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -3442,14 +3619,26 @@
       <c r="E71" t="s">
         <v>268</v>
       </c>
+      <c r="F71" t="s">
+        <v>321</v>
+      </c>
       <c r="G71" t="s">
         <v>266</v>
       </c>
+      <c r="H71" t="s">
+        <v>321</v>
+      </c>
       <c r="I71" t="s">
         <v>266</v>
       </c>
+      <c r="J71" t="s">
+        <v>321</v>
+      </c>
       <c r="K71" t="s">
         <v>266</v>
+      </c>
+      <c r="L71" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -3506,6 +3695,12 @@
       <c r="H73">
         <v>1</v>
       </c>
+      <c r="J73" t="s">
+        <v>321</v>
+      </c>
+      <c r="L73" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -3561,6 +3756,12 @@
       <c r="H75">
         <v>1</v>
       </c>
+      <c r="J75" t="s">
+        <v>321</v>
+      </c>
+      <c r="L75" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -3590,6 +3791,12 @@
       <c r="I76" t="s">
         <v>288</v>
       </c>
+      <c r="J76" t="s">
+        <v>321</v>
+      </c>
+      <c r="L76" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -3636,11 +3843,23 @@
       <c r="E78" t="s">
         <v>302</v>
       </c>
+      <c r="F78" t="s">
+        <v>321</v>
+      </c>
       <c r="G78" t="s">
         <v>301</v>
       </c>
+      <c r="H78" t="s">
+        <v>321</v>
+      </c>
       <c r="I78" t="s">
         <v>300</v>
+      </c>
+      <c r="J78" t="s">
+        <v>321</v>
+      </c>
+      <c r="L78" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
@@ -3659,11 +3878,23 @@
       <c r="E79" t="s">
         <v>304</v>
       </c>
+      <c r="F79" t="s">
+        <v>321</v>
+      </c>
       <c r="G79" t="s">
         <v>301</v>
       </c>
+      <c r="H79" t="s">
+        <v>321</v>
+      </c>
       <c r="I79" t="s">
         <v>300</v>
+      </c>
+      <c r="J79" t="s">
+        <v>321</v>
+      </c>
+      <c r="L79" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -3682,14 +3913,26 @@
       <c r="E80" t="s">
         <v>306</v>
       </c>
+      <c r="F80" t="s">
+        <v>321</v>
+      </c>
       <c r="G80" t="s">
         <v>301</v>
       </c>
+      <c r="H80" t="s">
+        <v>321</v>
+      </c>
       <c r="I80" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J80" t="s">
+        <v>321</v>
+      </c>
+      <c r="L80" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>308</v>
       </c>
@@ -3705,14 +3948,26 @@
       <c r="E81" t="s">
         <v>309</v>
       </c>
+      <c r="F81" t="s">
+        <v>321</v>
+      </c>
       <c r="G81" t="s">
         <v>301</v>
       </c>
+      <c r="H81" t="s">
+        <v>321</v>
+      </c>
       <c r="I81" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J81" t="s">
+        <v>321</v>
+      </c>
+      <c r="L81" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>311</v>
       </c>
@@ -3728,14 +3983,26 @@
       <c r="E82" t="s">
         <v>310</v>
       </c>
+      <c r="F82" t="s">
+        <v>321</v>
+      </c>
       <c r="G82" t="s">
         <v>301</v>
       </c>
+      <c r="H82" t="s">
+        <v>321</v>
+      </c>
       <c r="I82" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J82" t="s">
+        <v>321</v>
+      </c>
+      <c r="L82" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -3763,8 +4030,11 @@
       <c r="K83" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L83" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>56</v>
       </c>
@@ -3792,8 +4062,11 @@
       <c r="K84" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L84" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>57</v>
       </c>
@@ -3821,8 +4094,11 @@
       <c r="K85" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L85" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>318</v>
       </c>
@@ -3843,6 +4119,12 @@
       </c>
       <c r="H86">
         <v>2</v>
+      </c>
+      <c r="J86" t="s">
+        <v>321</v>
+      </c>
+      <c r="L86" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>